<commit_message>
Update: 33 product variations from Villages.fi with colors and sizes
</commit_message>
<xml_diff>
--- a/carpetfellows_tuotteet.xlsx
+++ b/carpetfellows_tuotteet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,35 +434,45 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Vari</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Koko</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Kuvaus</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Hinta</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Kategoria</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Varasto</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>KuvaURL</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>VillagesURL</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Materiaali</t>
         </is>
@@ -470,30 +480,44 @@
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Casandra</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+          <t>Beige/Multi</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Casandra on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>96</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Matto</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
         <is>
           <t>https://shop.villages.fi/tuote/casandra/</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -501,30 +525,44 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Casandra</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>96</v>
+          <t>Beige/Multi</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Casandra on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/agadir/</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+        <v>115</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/casandra/</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -532,123 +570,179 @@
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Casandra</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>31.4</v>
+          <t>Beige/Multi</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>160x230 cm</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Casandra on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/polku/</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>151</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/casandra/</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Agadir</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>31.4</v>
+          <t>Ruskea/Multi</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Agadir on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/eramaa/</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>96</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/agadir/</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Agadir</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>31.4</v>
+          <t>Ruskea/Multi</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Agadir on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/lapin-syksy/</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>115</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>10</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/agadir/</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Agadir</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>86</v>
+          <t>Ruskea/Multi</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>160x230 cm</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Agadir on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/cashmire-zara-299/</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+        <v>151</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/agadir/</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -656,30 +750,44 @@
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Polku</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>86</v>
+          <t>Harmaa</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>60x110 cm</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Polku on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/cashmire-cashmire-santiago-213/</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+        <v>31.4</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/polku/</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -687,30 +795,44 @@
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Polku</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>86</v>
+          <t>Harmaa</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Polku on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/cashmire-isla-73/</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+        <v>45</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/polku/</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -718,30 +840,44 @@
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Polku</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>86</v>
+          <t>Harmaa</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Polku on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/cashmire-nora-72/</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+        <v>59</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/polku/</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -749,30 +885,44 @@
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Erämaa</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>86</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>60x110 cm</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Erämaa on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/cashmire-petra-05/</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+        <v>31.4</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/eramaa/</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -780,280 +930,406 @@
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Erämaa</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>30</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Käytävämatto</t>
+          <t>Erämaa on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/linnea-kaytavamatto-musta/</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>45</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/eramaa/</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Erämaa</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>30</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Käytävämatto</t>
+          <t>Erämaa on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/linnea-kaytavamatto-harmaa/</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>59</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>10</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/eramaa/</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Lapin syksy</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>30</v>
+          <t>Ruskea</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>60x110 cm</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Käytävämatto</t>
+          <t>Lapin syksy on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>10</v>
-      </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/linnea-kaytavamatto-beige/</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>31.4</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/lapin-syksy/</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Lapin syksy</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>78</v>
+          <t>Ruskea</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Lapin syksy on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/adele-matto/</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>45</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>10</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/lapin-syksy/</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Lapin syksy</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>78</v>
+          <t>Ruskea</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Lapin syksy on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä.</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/aurora-matto/</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>59</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>10</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/lapin-syksy/</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Cashmire ZARA</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>133</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Cashmire ZARA tuo lämpöä ja tyyliä kotiisi. Ylellinen viskoosi tuo mattoon silkkiäistä kiiltoa.</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
-      </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/nuppu-matto/</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>86</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>10</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/cashmire-zara-299/</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Viskoosi</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Cashmire ZARA</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>87</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Cashmire ZARA tuo lämpöä ja tyyliä kotiisi. Ylellinen viskoosi tuo mattoon silkkiäistä kiiltoa.</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
-      </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/lohko-matto/</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Polyester/Microfiber</t>
+        <v>113</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>10</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/cashmire-zara-299/</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Viskoosi</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Cashmire ZARA</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Laadukas villa on luonnollinen ja lämmin valinta. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>179</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>160x230 cm</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Cashmire ZARA tuo lämpöä ja tyyliä kotiisi. Ylellinen viskoosi tuo mattoon silkkiäistä kiiltoa.</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>10</v>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/kuura-vaalean-harmaa/</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Villa</t>
+        <v>140</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>10</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/cashmire-zara-299/</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Viskoosi</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Linnea</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Laadukas villa on luonnollinen ja lämmin valinta. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>179</v>
+          <t>Musta</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>67x100 cm</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Linnea käytävämatto on käytännöllinen valinta eteiseen tai käytävälle.</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>10</v>
-      </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/kuura-pellava/</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Villa</t>
+        <v>30</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Käytävämatto</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>10</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/linnea-kaytavamatto-musta/</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
@@ -1061,34 +1337,44 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kaunis itämainen Sorrento</t>
+          <t>Linnea</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Kodikas ja elegantti Kaunis itämainen Sorrento sopii täydellisesti suomalaiseen kotiin. Laadukas villa on luonnollinen ja lämmin valinta. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>20</v>
+          <t>Musta</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>67x150 cm</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Linnea käytävämatto on käytännöllinen valinta eteiseen tai käytävälle.</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
-      </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/sorrento/</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Villa</t>
+        <v>45</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Käytävämatto</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>10</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/linnea-kaytavamatto-musta/</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
@@ -1096,125 +1382,177 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kaunis itämainen Alessia</t>
+          <t>Linnea</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Kaunis itämainen Alessia on ajaton valinta skandinaaviseen kotiin. Laadukas villa on luonnollinen ja lämmin valinta. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
+          <t>Musta</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>67x200 cm</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Linnea käytävämatto on käytännöllinen valinta eteiseen tai käytävälle.</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>10</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/alessia/</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Villa</t>
+        <v>61</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Käytävämatto</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>10</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/linnea-kaytavamatto-musta/</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Adele</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Ylellinen viskoosi tuo mattoon silkkiäistä kiiltoa. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>20</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>80x150 cm</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Adele yhdistää modernin muotoilun ja kestävän laadun.</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>10</v>
-      </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/lissabon-viskoosimatto/</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Viskoosi</t>
+        <v>78</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>10</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/adele-matto/</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Adele</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Ylellinen viskoosi tuo mattoon silkkiäistä kiiltoa. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>20</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Adele yhdistää modernin muotoilun ja kestävän laadun.</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>10</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/luxor-viskoosimatto/</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Viskoosi</t>
+        <v>99</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>10</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/adele-matto/</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Adele</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>30</v>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>160x230 cm</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Adele yhdistää modernin muotoilun ja kestävän laadun.</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>10</v>
-      </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/kanerva-beige/</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
+        <v>120</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>10</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/adele-matto/</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>Polyester</t>
         </is>
@@ -1222,32 +1560,46 @@
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Kuura</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>30</v>
+          <t>Vaalean harmaa</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Kuura on kodikas ja elegantti valinta suomalaiseen kotiin. Laadukas villa.</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
-      </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/kanerva-hopea/</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Polyester</t>
+        <v>179</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>10</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/kuura-vaalean-harmaa/</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Villa</t>
         </is>
       </c>
     </row>
@@ -1255,36 +1607,44 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Stockholm</t>
+          <t>Kuura</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Stockholm on ajaton valinta skandinaaviseen kotiin. Kevyt ja helppohoitoinen polyesteri kestää arjen käyttöä. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
+          <t>Vaalean harmaa</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>145.00</t>
+          <t>160x230 cm</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Kuura on kodikas ja elegantti valinta suomalaiseen kotiin. Laadukas villa.</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
-      </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/stockholm/</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Polyester</t>
+        <v>234</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/kuura-vaalean-harmaa/</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Villa</t>
         </is>
       </c>
     </row>
@@ -1292,34 +1652,42 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Helsinki</t>
+          <t>Kuura</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tuo lämpöä ja tyyliä kotiisi Helsinki-matolla. Käytännöllinen materiaali sopii aktiiviseen arkeen. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
+          <t>Vaalean harmaa</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>189.00</t>
+          <t>200x290 cm</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Kuura on kodikas ja elegantti valinta suomalaiseen kotiin. Laadukas villa.</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
-      </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/helsinki/</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
+        <v>289</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>10</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/kuura-vaalean-harmaa/</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>Villa</t>
         </is>
@@ -1329,36 +1697,44 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Oslo</t>
+          <t>Sorrento</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Oslo yhdistää modernin muotoilun ja kestävän laadun. Laadukas villa on luonnollinen ja lämmin valinta. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
+          <t>Punainen</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>220.00</t>
+          <t>80x150 cm</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Sorrento tuo lämpöä ja tyyliä kotiisi. Kaunis itämainen kuviointi.</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>10</v>
-      </c>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/oslo/</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Villa</t>
+        <v>91</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>10</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/sorrento/</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
@@ -1366,36 +1742,44 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Kööpenhamina</t>
+          <t>Sorrento</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Kodikas ja elegantti Kööpenhamina sopii täydellisesti suomalaiseen kotiin. Ylellinen viskoosi tuo mattoon silkkiäistä kiiltoa. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
+          <t>Punainen</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>165.00</t>
+          <t>120x170 cm</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Viskoosimatto</t>
+          <t>Sorrento tuo lämpöä ja tyyliä kotiisi. Kaunis itämainen kuviointi.</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>10</v>
-      </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/kööpenhamina/</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Viskoosi</t>
+        <v>120</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>10</v>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/sorrento/</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Polyester</t>
         </is>
       </c>
     </row>
@@ -1403,36 +1787,179 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tukholma</t>
+          <t>Kanerva</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Tukholma on ajaton valinta skandinaaviseen kotiin. Pehmeä puuvilla on miellyttävä jalan alla. Imuroi säännöllisesti ja puhdista tahrat välittömästi.</t>
+          <t>Beige</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>125.00</t>
+          <t>80x150 cm</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Matto</t>
+          <t>Kanerva on ajaton valinta skandinaaviseen kotiin. Pehmeä puuvilla.</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>10</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>https://shop.villages.fi/tuote/tukholma/</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
+        <v>55</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>10</v>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/kanerva-beige/</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>Puuvilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Kanerva</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Kanerva on ajaton valinta skandinaaviseen kotiin. Pehmeä puuvilla.</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>87</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Matto</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>10</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/kanerva-beige/</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Puuvilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Lissabon</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Harmaa</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>120x170 cm</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Lissabon tuo ylellistä kiiltoa kotiisi. Viskoosi on elegantti valinta.</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>109</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Viskoosimatto</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>10</v>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/lissabon-viskoosimatto/</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Viskoosi</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Lissabon</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Harmaa</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>160x230 cm</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Lissabon tuo ylellistä kiiltoa kotiisi. Viskoosi on elegantti valinta.</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>174</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Viskoosimatto</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>10</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>https://shop.villages.fi/tuote/lissabon-viskoosimatto/</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Viskoosi</t>
         </is>
       </c>
     </row>

</xml_diff>